<commit_message>
Data checks with thests, hopefully done
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data_tests.xlsx
+++ b/tests/testthat/testdata/data_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012016E1-A7CA-4A2E-9F66-AA18606BE11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1614DD-9F1D-4138-8AF5-6E219C3C8AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1950" windowWidth="23700" windowHeight="13440" activeTab="10" xr2:uid="{D97F5896-51C5-4041-8CB0-0334D423D4AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="10" xr2:uid="{D97F5896-51C5-4041-8CB0-0334D423D4AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t xml:space="preserve">period </t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>UMAR--MZ007--LKJ--1999--A</t>
+  </si>
+  <si>
+    <t>UMAR--MZ002--12dfg--M</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +514,7 @@
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,57 +566,69 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0654B8E1-628B-487D-A0EB-DE609E777C19}">
-  <dimension ref="C3:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D070EA5-22F5-495B-8495-4619F6BEFF1C}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D1" sqref="D1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>212</v>
+      </c>
+      <c r="C3">
+        <v>221</v>
+      </c>
+      <c r="D3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>213</v>
+      </c>
       <c r="C4">
-        <v>2021</v>
+        <v>112</v>
       </c>
       <c r="D4">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>2022</v>
-      </c>
-      <c r="D5">
-        <v>212</v>
-      </c>
-      <c r="E5">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>1999</v>
-      </c>
-      <c r="D6">
-        <v>213</v>
-      </c>
-      <c r="E6">
-        <v>213</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -625,7 +640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E502D08F-949E-436E-95E3-DD69B413B67F}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -807,7 +824,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +883,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1036,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>